<commit_message>
mior modifications to some xlsx and progress in wrangling nfishers data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/Table4.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/Table4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb111/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9642A5C5-D313-B943-A8FB-B6276D160DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CB6310-7CB1-BA42-8A4F-EEF510648915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Area of residence</t>
   </si>
@@ -41,12 +41,6 @@
     <t>1959-1960</t>
   </si>
   <si>
-    <t>Santa Barbara____</t>
-  </si>
-  <si>
-    <t>Mexican nationals licensed in California____________________________ _</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eureka  </t>
   </si>
   <si>
@@ -69,6 +63,18 @@
   </si>
   <si>
     <t>Total check</t>
+  </si>
+  <si>
+    <t>Santa Barbara</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>Mexican nationals licensed in California</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -146,17 +152,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -475,7 +481,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,7 +506,7 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="6">
         <v>922</v>
@@ -511,7 +517,7 @@
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="7">
         <v>115</v>
@@ -522,7 +528,7 @@
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6">
         <v>1069</v>
@@ -533,7 +539,7 @@
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="7">
         <v>777</v>
@@ -544,7 +550,7 @@
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7">
         <v>535</v>
@@ -554,7 +560,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="6">
         <v>2517</v>
       </c>
@@ -563,7 +571,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="6">
         <v>2122</v>
       </c>
@@ -573,7 +583,7 @@
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6">
         <v>486</v>
@@ -582,9 +592,9 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6">
         <v>16</v>
@@ -595,7 +605,7 @@
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8">
         <v>11</v>
@@ -606,7 +616,7 @@
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="7">
         <v>8570</v>
@@ -617,7 +627,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="10">
         <f>SUM(B2:B11)-B12</f>

</xml_diff>